<commit_message>
have to handle special characters when writing to xl sheet
</commit_message>
<xml_diff>
--- a/main/example5.xlsx
+++ b/main/example5.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Buoyancy</t>
   </si>
@@ -57,12 +57,6 @@
   </si>
   <si>
     <t>Flotation</t>
-  </si>
-  <si>
-    <t>WB-17                         </t>
-  </si>
-  <si>
-    <t>AF44�� w WH150+SBE37 ODO     </t>
   </si>
 </sst>
 </file>
@@ -380,7 +374,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -423,16 +417,6 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>